<commit_message>
decision table support added
</commit_message>
<xml_diff>
--- a/src/main/resources/authorization-rules/access-decision-table.xlsx
+++ b/src/main/resources/authorization-rules/access-decision-table.xlsx
@@ -891,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H19"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -910,163 +910,182 @@
     <col min="10" max="10" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-    </row>
-    <row r="4" spans="1:7" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+    <row r="6" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+    <row r="9" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C10" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D10" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E10" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F10" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G10" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="11" spans="1:7" ht="45" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G11" s="13" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
         <v>0</v>
       </c>
@@ -1074,18 +1093,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="F14" s="5" t="s">
         <v>0</v>
       </c>
@@ -1095,16 +1118,16 @@
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>0</v>
@@ -1118,16 +1141,16 @@
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>0</v>
@@ -1141,16 +1164,16 @@
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
-        <v>5</v>
-      </c>
-      <c r="B17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>75</v>
+        <v>13</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>0</v>
@@ -1162,18 +1185,18 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>0</v>
@@ -1182,84 +1205,55 @@
         <v>0</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>7</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" s="12" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="2">
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>tables!$H$2:$H$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B13:B28 C20:D28</xm:sqref>
+          <xm:sqref>B12:B27 C19:D27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>tables!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G21:G35 F20:F35</xm:sqref>
+          <xm:sqref>G20:G34 F19:F34</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>tables!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G20</xm:sqref>
+          <xm:sqref>G19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>tables!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E13:F19 H20:I20 I13:I19 C1:E1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>tables!$A$12:$A$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1</xm:sqref>
+          <xm:sqref>E12:F18 H19:I19 I12:I18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>tables!$A$2:$A$113</xm:f>
           </x14:formula1>
-          <xm:sqref>E20:E43 C13:C19</xm:sqref>
+          <xm:sqref>E19:E42 C12:C18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>tables!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D13:D19</xm:sqref>
+          <xm:sqref>D12:D18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
decision table bug fix
</commit_message>
<xml_diff>
--- a/src/main/resources/authorization-rules/access-decision-table.xlsx
+++ b/src/main/resources/authorization-rules/access-decision-table.xlsx
@@ -265,13 +265,13 @@
     <t xml:space="preserve">assessment.status == AssessmentStatus.$param </t>
   </si>
   <si>
-    <t>user.countyCwsCode == assessment.county.externalId &amp;&amp; "$param" == "Yes"</t>
-  </si>
-  <si>
     <t>assessmentAccessible &amp;&amp; "$param" == "Yes"</t>
   </si>
   <si>
     <t>gov.ca.cwds.cans.security.assessment.facts.AssessmentOperationFact, java.lang.Boolean, gov.ca.cwds.cans.domain.enumeration.AssessmentStatus, gov.ca.cwds.cans.security.assessment.AssessmentOperation, gov.ca.cwds.security.realm.PerryAccount, gov.ca.cwds.cans.domain.entity.Assessment</t>
+  </si>
+  <si>
+    <t>user.countyCwsCode == assessment.person.county.externalId &amp;&amp; "$param" == "Yes"</t>
   </si>
 </sst>
 </file>
@@ -905,7 +905,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -948,7 +948,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -1033,10 +1033,10 @@
         <v>78</v>
       </c>
       <c r="E10" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>80</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
decision table: rule: complete new assessment
</commit_message>
<xml_diff>
--- a/src/main/resources/authorization-rules/access-decision-table.xlsx
+++ b/src/main/resources/authorization-rules/access-decision-table.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="83">
   <si>
     <t>Yes</t>
   </si>
@@ -262,9 +262,6 @@
     <t>user.privileges contains "$param"</t>
   </si>
   <si>
-    <t xml:space="preserve">assessment.status == AssessmentStatus.$param </t>
-  </si>
-  <si>
     <t>assessmentAccessible &amp;&amp; "$param" == "Yes"</t>
   </si>
   <si>
@@ -272,6 +269,12 @@
   </si>
   <si>
     <t>(assessment.person.county == null || user.countyCwsCode == assessment.person.county.externalId) &amp;&amp; "$param" == "Yes"</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eval( ("NEW".equals("$param") &amp;&amp;  assessment.getStatus() == null) || (! "NEW".equals("$param") &amp;&amp; assessment.getStatus() == AssessmentStatus.valueOf("$param"))) </t>
   </si>
 </sst>
 </file>
@@ -902,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -948,7 +951,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -1022,7 +1025,7 @@
       <c r="F9" s="21"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="105" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
         <v>75</v>
       </c>
@@ -1030,13 +1033,13 @@
         <v>77</v>
       </c>
       <c r="D10" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>78</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>79</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>66</v>
@@ -1217,6 +1220,29 @@
         <v>0</v>
       </c>
       <c r="G18" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1230,42 +1256,36 @@
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>tables!$H$2:$H$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B12:B27 C19:D27</xm:sqref>
+          <xm:sqref>C20:D27 B12:B27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>tables!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G20:G34 F19:F34</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>tables!$G$2:$G$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>G19</xm:sqref>
+          <xm:sqref>F20:G34</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>tables!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E12:F18 H19:I19 I12:I18</xm:sqref>
+          <xm:sqref>E12:F19 I12:I19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>tables!$A$2:$A$113</xm:f>
           </x14:formula1>
-          <xm:sqref>E19:E42 C12:C18</xm:sqref>
+          <xm:sqref>C12:C19 E20:E42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>tables!$B$2:$B$4</xm:f>
+            <xm:f>tables!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D12:D18</xm:sqref>
+          <xm:sqref>D12:D19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1277,7 +1297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1502,7 +1522,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,6 +1650,9 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
       <c r="H5" t="s">
         <v>73</v>
       </c>

</xml_diff>